<commit_message>
Merging and bug fixes
</commit_message>
<xml_diff>
--- a/Project Planning/CS 270 Project Planning.xlsx
+++ b/Project Planning/CS 270 Project Planning.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bbgri\Documents\GitHub\RoanokeMobileOrdering\Project Planning\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{56DB85AA-7D28-4603-A153-187FAEBDCBD2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BB9BF99A-17D6-4394-B15C-1F1DD902BD28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-103" yWindow="-103" windowWidth="22149" windowHeight="11949" xr2:uid="{88243482-28B6-4BDC-8B56-680E2E2A9CC5}"/>
   </bookViews>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="27">
   <si>
     <t>Nutrition Info</t>
   </si>
@@ -110,6 +110,12 @@
   </si>
   <si>
     <t>ID:</t>
+  </si>
+  <si>
+    <t>Tab Bar</t>
+  </si>
+  <si>
+    <t>Checkout</t>
   </si>
 </sst>
 </file>
@@ -125,7 +131,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -135,6 +141,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -151,9 +163,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -468,10 +481,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D57020BF-FBC2-4E0B-ADBC-9B415A80F232}">
-  <dimension ref="A1:D22"/>
+  <dimension ref="A1:D24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="A24" sqref="A24:D24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
@@ -495,106 +508,106 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A2">
+      <c r="A2" s="1">
         <v>1</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C2">
-        <v>10</v>
-      </c>
-      <c r="D2">
+      <c r="C2" s="1">
+        <v>10</v>
+      </c>
+      <c r="D2" s="1">
         <v>3</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A3">
+      <c r="A3" s="1">
         <f>A2+1</f>
         <v>2</v>
       </c>
-      <c r="B3" t="s">
+      <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C3">
-        <v>10</v>
-      </c>
-      <c r="D3">
+      <c r="C3" s="1">
+        <v>10</v>
+      </c>
+      <c r="D3" s="1">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A4">
+      <c r="A4" s="1">
         <f t="shared" ref="A4:A22" si="0">A3+1</f>
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>2</v>
-      </c>
-      <c r="C4">
-        <v>10</v>
-      </c>
-      <c r="D4">
+      <c r="B4" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C4" s="1">
+        <v>10</v>
+      </c>
+      <c r="D4" s="1">
         <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A5">
+      <c r="A5" s="1">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B5" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="C5">
+      <c r="C5" s="1">
         <v>8</v>
       </c>
-      <c r="D5">
+      <c r="D5" s="1">
         <v>2</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A6">
+      <c r="A6" s="1">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C6">
-        <v>10</v>
-      </c>
-      <c r="D6">
+      <c r="C6" s="1">
+        <v>10</v>
+      </c>
+      <c r="D6" s="1">
         <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A7">
+      <c r="A7" s="1">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C7">
-        <v>10</v>
-      </c>
-      <c r="D7">
+      <c r="C7" s="1">
+        <v>10</v>
+      </c>
+      <c r="D7" s="1">
         <v>2</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A8">
+      <c r="A8" s="1">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B8" t="s">
+      <c r="B8" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="C8">
-        <v>10</v>
-      </c>
-      <c r="D8">
+      <c r="C8" s="1">
+        <v>10</v>
+      </c>
+      <c r="D8" s="1">
         <v>2</v>
       </c>
     </row>
@@ -644,17 +657,17 @@
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.4">
-      <c r="A12">
+      <c r="A12" s="2">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="B12" t="s">
-        <v>10</v>
-      </c>
-      <c r="C12">
+      <c r="B12" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="C12" s="2">
         <v>7</v>
       </c>
-      <c r="D12">
+      <c r="D12" s="2">
         <v>8</v>
       </c>
     </row>
@@ -806,6 +819,34 @@
       </c>
       <c r="D22">
         <v>4</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A23" s="2">
+        <v>22</v>
+      </c>
+      <c r="B23" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C23" s="2">
+        <v>10</v>
+      </c>
+      <c r="D23" s="2">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" t="s">
+        <v>26</v>
+      </c>
+      <c r="C24">
+        <v>10</v>
+      </c>
+      <c r="D24">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>